<commit_message>
shiny app, got histogram, country and side layouts
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ACE69EB-3CBD-4CAF-8399-2EBD5E34DAB4}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1FFF66E-0CB5-4E5D-84AB-B9C93E98F987}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Date and time</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Worked on minidemo, timelog and calendar</t>
+  </si>
+  <si>
+    <t>2/22, 3 hours</t>
+  </si>
+  <si>
+    <t>Worked on shiny app, adding histogram and side layouts</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +672,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
second map and clicker
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1FFF66E-0CB5-4E5D-84AB-B9C93E98F987}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF2F3746-26DC-40D0-B516-4B6D60749326}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Date and time</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>Worked on shiny app, adding histogram and side layouts</t>
+  </si>
+  <si>
+    <t>2/23, 2 hours</t>
+  </si>
+  <si>
+    <t>worked on click output and brush output</t>
+  </si>
+  <si>
+    <t>Worked on second map which zooms in, adding clicker for second map</t>
   </si>
 </sst>
 </file>
@@ -535,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,6 +689,22 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
prepped for presentation and reorganized
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF2F3746-26DC-40D0-B516-4B6D60749326}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B505C7-3DCD-493A-8968-026D3E6687D6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Date and time</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Worked on second map which zooms in, adding clicker for second map</t>
+  </si>
+  <si>
+    <t>2/23, 2 hours (4 total)</t>
+  </si>
+  <si>
+    <t>2/24, 45 mins</t>
+  </si>
+  <si>
+    <t>Worked on reorganizing app, taking pics for presentation</t>
   </si>
 </sst>
 </file>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,10 +708,18 @@
     </row>
     <row r="18" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WDD work, lat long, works until today
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B505C7-3DCD-493A-8968-026D3E6687D6}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9274A2CF-2E44-461F-AD6F-CBAA1913A52A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Date and time</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>Worked on reorganizing app, taking pics for presentation</t>
+  </si>
+  <si>
+    <t>3/1, 1hr</t>
+  </si>
+  <si>
+    <t>working on getting shiny app to work until today</t>
+  </si>
+  <si>
+    <t>3/2, 30 mins</t>
+  </si>
+  <si>
+    <t>testing covid overtime graph</t>
   </si>
 </sst>
 </file>
@@ -553,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,6 +734,22 @@
         <v>37</v>
       </c>
     </row>
+    <row r="20" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding fourth visualization and testing
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F3BE529-F21C-4C17-B701-A61FF58CE91B}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AF7094F-4857-4CD4-899C-688920F01530}"/>
   <bookViews>
     <workbookView xWindow="5736" yWindow="2568" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Date and time</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>working on making graph over time of clicked on country</t>
+  </si>
+  <si>
+    <t>Working on graph over time for country, addinggoverment to said graph</t>
+  </si>
+  <si>
+    <t>3/9, 4 hrs</t>
   </si>
 </sst>
 </file>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,6 +798,14 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding govt info to shiny, making things faster, fixing errors, docuementing
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AF7094F-4857-4CD4-899C-688920F01530}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67989421-58BD-4A94-BD86-C8CFCC2FED67}"/>
   <bookViews>
     <workbookView xWindow="5736" yWindow="2568" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Date and time</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>3/9, 4 hrs</t>
+  </si>
+  <si>
+    <t>3/10, 4 hrs</t>
+  </si>
+  <si>
+    <t>Working on adding govt measures to graphs, documenting, fixing errors, prepping final product</t>
   </si>
 </sst>
 </file>
@@ -589,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,6 +812,14 @@
         <v>48</v>
       </c>
     </row>
+    <row r="26" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
worked on shiny, documenting, cleaning graphs
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67989421-58BD-4A94-BD86-C8CFCC2FED67}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{229805EC-1C55-40B6-BDF4-F973F0CA40EE}"/>
   <bookViews>
-    <workbookView xWindow="5736" yWindow="2568" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Date and time</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Working on adding govt measures to graphs, documenting, fixing errors, prepping final product</t>
+  </si>
+  <si>
+    <t>3/11, 3 hrs</t>
+  </si>
+  <si>
+    <t>Work on govt data in shiny, documenting, cleaning up graphs</t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,6 +826,14 @@
         <v>51</v>
       </c>
     </row>
+    <row r="27" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working on final changes
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{229805EC-1C55-40B6-BDF4-F973F0CA40EE}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3186D25F-BD81-4B60-B21F-E23EDAE12AB4}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Date and time</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Work on govt data in shiny, documenting, cleaning up graphs</t>
+  </si>
+  <si>
+    <t>3/12, 4 hrs</t>
+  </si>
+  <si>
+    <t>Making things pretty, documenting, organizing, adding final touches</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,6 +840,14 @@
         <v>53</v>
       </c>
     </row>
+    <row r="28" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
final changes, documentation prettying of data, timelog
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/CSC324-repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3186D25F-BD81-4B60-B21F-E23EDAE12AB4}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{6B3B7DDF-3344-4CDB-81B2-9A374AE52FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E3737E-47B3-4EB9-AAE5-5ED0F6F6662D}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17304" windowHeight="9144" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3867AD3C-DAB3-4B8A-8114-C94099F923ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Date and time</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Making things pretty, documenting, organizing, adding final touches</t>
+  </si>
+  <si>
+    <t>3/13, 5 hrs</t>
+  </si>
+  <si>
+    <t>Final touches, documenting, recording video, making presentation</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD2AB1-2C8C-44DA-A9C8-BDAF964DE5C1}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,6 +854,14 @@
         <v>55</v>
       </c>
     </row>
+    <row r="29" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>